<commit_message>
4 new spreadsheets an update to the web page and an update to the spreadsheet template
</commit_message>
<xml_diff>
--- a/test-results/cloudreader/spreadsheets/duanwalker-Win7-chrome-20160129.xlsx
+++ b/test-results/cloudreader/spreadsheets/duanwalker-Win7-chrome-20160129.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="0" windowWidth="25035" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="705" yWindow="0" windowWidth="25035" windowHeight="13410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="734">
   <si>
     <t>epub30-test-0100.epub</t>
   </si>
@@ -2227,6 +2227,15 @@
   </si>
   <si>
     <t>The slideshow binding was not called</t>
+  </si>
+  <si>
+    <t>test does not exist</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>not supported</t>
   </si>
 </sst>
 </file>
@@ -2870,8 +2879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E500"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C138" sqref="C138"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C463" sqref="C463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -3155,11 +3164,11 @@
       </c>
       <c r="B28" s="31">
         <f>SUM(C111:C153)</f>
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C28" s="23">
         <f>B28/43</f>
-        <v>0.62790697674418605</v>
+        <v>0.79069767441860461</v>
       </c>
       <c r="D28" s="10"/>
     </row>
@@ -3169,11 +3178,11 @@
       </c>
       <c r="B29" s="31">
         <f>SUM(C161:C208)</f>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C29" s="23">
         <f>B29/56</f>
-        <v>0</v>
+        <v>0.8214285714285714</v>
       </c>
       <c r="D29" s="10"/>
     </row>
@@ -3183,11 +3192,11 @@
       </c>
       <c r="B30" s="31">
         <f>SUM(C216:C228)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C30" s="23">
         <f>B30/13</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="10"/>
     </row>
@@ -3197,11 +3206,11 @@
       </c>
       <c r="B31" s="31">
         <f>SUM(C235,C242,C249)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C31" s="23">
         <f>B31/3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="10"/>
     </row>
@@ -3211,11 +3220,11 @@
       </c>
       <c r="B32" s="31">
         <f>SUM(C256:C283)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C32" s="23">
         <f>B32/28</f>
-        <v>0</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="D32" s="10"/>
     </row>
@@ -3225,11 +3234,11 @@
       </c>
       <c r="B33" s="31">
         <f>SUM(C290:C331)</f>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C33" s="23">
         <f>B33/42</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="10"/>
     </row>
@@ -3239,11 +3248,11 @@
       </c>
       <c r="B34" s="31">
         <f>SUM(C339:C344,C346)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C34" s="23">
         <f>B34/7</f>
-        <v>0</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="D34" s="10"/>
     </row>
@@ -3253,11 +3262,11 @@
       </c>
       <c r="B35" s="31">
         <f>SUM(C353:C364)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C35" s="23">
         <f>B35/12</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D35" s="10"/>
     </row>
@@ -3267,11 +3276,11 @@
       </c>
       <c r="B36" s="31">
         <f>SUM(C371,C378,C385,C392,C399,C406,C413,C420,C427,C434,C435,C442,C443,C444,C445)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C36" s="23">
         <f>B36/15</f>
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D36" s="10"/>
     </row>
@@ -3281,11 +3290,11 @@
       </c>
       <c r="B37" s="31">
         <f>SUM(C452:C461)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C37" s="23">
         <f>B37/10</f>
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D37" s="10"/>
     </row>
@@ -3309,11 +3318,11 @@
       </c>
       <c r="B39" s="31">
         <f>SUM(B27:B38)</f>
-        <v>72</v>
+        <v>234</v>
       </c>
       <c r="C39" s="23">
         <f>B39/304</f>
-        <v>0.23684210526315788</v>
+        <v>0.76973684210526316</v>
       </c>
       <c r="D39" s="10"/>
     </row>
@@ -4668,7 +4677,9 @@
       <c r="B138" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C138" s="4"/>
+      <c r="C138" s="4">
+        <v>1</v>
+      </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4" t="s">
         <v>489</v>
@@ -4681,7 +4692,9 @@
       <c r="B139" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C139" s="4"/>
+      <c r="C139" s="4">
+        <v>1</v>
+      </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4" t="s">
         <v>490</v>
@@ -4694,8 +4707,12 @@
       <c r="B140" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C140" s="4"/>
-      <c r="D140" s="4"/>
+      <c r="C140" s="4">
+        <v>0</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>731</v>
+      </c>
       <c r="E140" s="4" t="s">
         <v>491</v>
       </c>
@@ -4707,8 +4724,12 @@
       <c r="B141" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C141" s="4"/>
-      <c r="D141" s="4"/>
+      <c r="C141" s="4">
+        <v>0</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>731</v>
+      </c>
       <c r="E141" s="4" t="s">
         <v>492</v>
       </c>
@@ -4720,7 +4741,9 @@
       <c r="B142" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C142" s="4"/>
+      <c r="C142" s="4">
+        <v>1</v>
+      </c>
       <c r="D142" s="4"/>
       <c r="E142" s="4" t="s">
         <v>493</v>
@@ -4733,8 +4756,12 @@
       <c r="B143" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C143" s="4"/>
-      <c r="D143" s="4"/>
+      <c r="C143" s="4">
+        <v>0</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>732</v>
+      </c>
       <c r="E143" s="4" t="s">
         <v>494</v>
       </c>
@@ -4746,8 +4773,12 @@
       <c r="B144" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C144" s="4"/>
-      <c r="D144" s="4"/>
+      <c r="C144" s="4">
+        <v>0</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>731</v>
+      </c>
       <c r="E144" s="4" t="s">
         <v>495</v>
       </c>
@@ -4759,8 +4790,12 @@
       <c r="B145" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C145" s="4"/>
-      <c r="D145" s="4"/>
+      <c r="C145" s="4">
+        <v>0</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>731</v>
+      </c>
       <c r="E145" s="4" t="s">
         <v>496</v>
       </c>
@@ -4772,8 +4807,12 @@
       <c r="B146" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C146" s="4"/>
-      <c r="D146" s="4"/>
+      <c r="C146" s="4">
+        <v>0</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>731</v>
+      </c>
       <c r="E146" s="4" t="s">
         <v>497</v>
       </c>
@@ -4785,8 +4824,12 @@
       <c r="B147" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C147" s="4"/>
-      <c r="D147" s="4"/>
+      <c r="C147" s="4">
+        <v>0</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>731</v>
+      </c>
       <c r="E147" s="4" t="s">
         <v>498</v>
       </c>
@@ -4798,7 +4841,9 @@
       <c r="B148" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C148" s="4"/>
+      <c r="C148" s="4">
+        <v>1</v>
+      </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4" t="s">
         <v>499</v>
@@ -4811,7 +4856,9 @@
       <c r="B149" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C149" s="4"/>
+      <c r="C149" s="4">
+        <v>1</v>
+      </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4" t="s">
         <v>500</v>
@@ -4824,7 +4871,9 @@
       <c r="B150" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C150" s="4"/>
+      <c r="C150" s="4">
+        <v>1</v>
+      </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4" t="s">
         <v>501</v>
@@ -4837,7 +4886,9 @@
       <c r="B151" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C151" s="4"/>
+      <c r="C151" s="4">
+        <v>1</v>
+      </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4" t="s">
         <v>502</v>
@@ -4850,7 +4901,9 @@
       <c r="B152" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C152" s="4"/>
+      <c r="C152" s="4">
+        <v>0</v>
+      </c>
       <c r="D152" s="4"/>
       <c r="E152" s="4" t="s">
         <v>503</v>
@@ -4863,7 +4916,9 @@
       <c r="B153" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C153" s="4"/>
+      <c r="C153" s="4">
+        <v>0</v>
+      </c>
       <c r="D153" s="4"/>
       <c r="E153" s="4" t="s">
         <v>504</v>
@@ -4912,7 +4967,9 @@
       <c r="B161" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C161" s="4"/>
+      <c r="C161" s="4">
+        <v>1</v>
+      </c>
       <c r="D161" s="4"/>
       <c r="E161" s="4" t="s">
         <v>505</v>
@@ -4925,7 +4982,9 @@
       <c r="B162" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C162" s="4"/>
+      <c r="C162" s="4">
+        <v>1</v>
+      </c>
       <c r="D162" s="4"/>
       <c r="E162" s="4" t="s">
         <v>506</v>
@@ -4938,7 +4997,9 @@
       <c r="B163" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C163" s="4"/>
+      <c r="C163" s="4">
+        <v>1</v>
+      </c>
       <c r="D163" s="4"/>
       <c r="E163" s="4" t="s">
         <v>507</v>
@@ -4951,7 +5012,9 @@
       <c r="B164" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C164" s="4"/>
+      <c r="C164" s="4">
+        <v>1</v>
+      </c>
       <c r="D164" s="4"/>
       <c r="E164" s="4" t="s">
         <v>508</v>
@@ -4964,7 +5027,9 @@
       <c r="B165" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C165" s="4"/>
+      <c r="C165" s="4">
+        <v>1</v>
+      </c>
       <c r="D165" s="4"/>
       <c r="E165" s="4" t="s">
         <v>509</v>
@@ -4977,7 +5042,9 @@
       <c r="B166" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C166" s="4"/>
+      <c r="C166" s="4">
+        <v>1</v>
+      </c>
       <c r="D166" s="4"/>
       <c r="E166" s="4" t="s">
         <v>510</v>
@@ -4990,8 +5057,12 @@
       <c r="B167" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C167" s="4"/>
-      <c r="D167" s="4"/>
+      <c r="C167" s="4">
+        <v>0</v>
+      </c>
+      <c r="D167" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="E167" s="4" t="s">
         <v>511</v>
       </c>
@@ -5003,7 +5074,9 @@
       <c r="B168" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C168" s="4"/>
+      <c r="C168" s="4">
+        <v>1</v>
+      </c>
       <c r="D168" s="4"/>
       <c r="E168" s="4" t="s">
         <v>512</v>
@@ -5016,7 +5089,9 @@
       <c r="B169" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C169" s="4"/>
+      <c r="C169" s="4">
+        <v>1</v>
+      </c>
       <c r="D169" s="4"/>
       <c r="E169" s="4" t="s">
         <v>513</v>
@@ -5029,7 +5104,9 @@
       <c r="B170" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C170" s="4"/>
+      <c r="C170" s="4">
+        <v>1</v>
+      </c>
       <c r="D170" s="4"/>
       <c r="E170" s="4" t="s">
         <v>514</v>
@@ -5042,7 +5119,9 @@
       <c r="B171" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C171" s="4"/>
+      <c r="C171" s="4">
+        <v>1</v>
+      </c>
       <c r="D171" s="4"/>
       <c r="E171" s="4" t="s">
         <v>515</v>
@@ -5055,7 +5134,9 @@
       <c r="B172" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C172" s="4"/>
+      <c r="C172" s="4">
+        <v>1</v>
+      </c>
       <c r="D172" s="4"/>
       <c r="E172" s="4" t="s">
         <v>134</v>
@@ -5068,8 +5149,12 @@
       <c r="B173" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C173" s="4"/>
-      <c r="D173" s="4"/>
+      <c r="C173" s="4">
+        <v>0</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>732</v>
+      </c>
       <c r="E173" s="4" t="s">
         <v>136</v>
       </c>
@@ -5081,7 +5166,9 @@
       <c r="B174" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C174" s="4"/>
+      <c r="C174" s="4">
+        <v>1</v>
+      </c>
       <c r="D174" s="4"/>
       <c r="E174" s="4" t="s">
         <v>516</v>
@@ -5094,7 +5181,9 @@
       <c r="B175" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C175" s="4"/>
+      <c r="C175" s="4">
+        <v>1</v>
+      </c>
       <c r="D175" s="4"/>
       <c r="E175" s="4" t="s">
         <v>139</v>
@@ -5107,7 +5196,9 @@
       <c r="B176" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C176" s="4"/>
+      <c r="C176" s="4">
+        <v>1</v>
+      </c>
       <c r="D176" s="4"/>
       <c r="E176" s="4" t="s">
         <v>517</v>
@@ -5120,7 +5211,9 @@
       <c r="B177" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C177" s="4"/>
+      <c r="C177" s="4">
+        <v>1</v>
+      </c>
       <c r="D177" s="4"/>
       <c r="E177" s="4" t="s">
         <v>142</v>
@@ -5133,7 +5226,9 @@
       <c r="B178" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C178" s="4"/>
+      <c r="C178" s="4">
+        <v>1</v>
+      </c>
       <c r="D178" s="4"/>
       <c r="E178" s="4" t="s">
         <v>518</v>
@@ -5146,7 +5241,9 @@
       <c r="B179" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C179" s="4"/>
+      <c r="C179" s="4">
+        <v>1</v>
+      </c>
       <c r="D179" s="4"/>
       <c r="E179" s="4" t="s">
         <v>519</v>
@@ -5159,7 +5256,9 @@
       <c r="B180" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C180" s="4"/>
+      <c r="C180" s="4">
+        <v>1</v>
+      </c>
       <c r="D180" s="4"/>
       <c r="E180" s="4" t="s">
         <v>146</v>
@@ -5172,7 +5271,9 @@
       <c r="B181" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C181" s="4"/>
+      <c r="C181" s="4">
+        <v>1</v>
+      </c>
       <c r="D181" s="4"/>
       <c r="E181" s="4" t="s">
         <v>148</v>
@@ -5185,7 +5286,9 @@
       <c r="B182" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C182" s="4"/>
+      <c r="C182" s="4">
+        <v>1</v>
+      </c>
       <c r="D182" s="4"/>
       <c r="E182" s="4" t="s">
         <v>150</v>
@@ -5198,7 +5301,9 @@
       <c r="B183" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C183" s="4"/>
+      <c r="C183" s="4">
+        <v>1</v>
+      </c>
       <c r="D183" s="4"/>
       <c r="E183" s="4" t="s">
         <v>520</v>
@@ -5211,7 +5316,9 @@
       <c r="B184" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C184" s="4"/>
+      <c r="C184" s="4">
+        <v>1</v>
+      </c>
       <c r="D184" s="4"/>
       <c r="E184" s="4" t="s">
         <v>521</v>
@@ -5224,7 +5331,9 @@
       <c r="B185" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C185" s="4"/>
+      <c r="C185" s="4">
+        <v>1</v>
+      </c>
       <c r="D185" s="4"/>
       <c r="E185" s="4" t="s">
         <v>522</v>
@@ -5237,7 +5346,9 @@
       <c r="B186" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C186" s="4"/>
+      <c r="C186" s="4">
+        <v>1</v>
+      </c>
       <c r="D186" s="4"/>
       <c r="E186" s="4" t="s">
         <v>523</v>
@@ -5250,7 +5361,9 @@
       <c r="B187" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C187" s="4"/>
+      <c r="C187" s="4">
+        <v>1</v>
+      </c>
       <c r="D187" s="4"/>
       <c r="E187" s="4" t="s">
         <v>524</v>
@@ -5263,7 +5376,9 @@
       <c r="B188" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C188" s="4"/>
+      <c r="C188" s="4">
+        <v>1</v>
+      </c>
       <c r="D188" s="4"/>
       <c r="E188" s="4" t="s">
         <v>525</v>
@@ -5276,7 +5391,9 @@
       <c r="B189" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C189" s="4"/>
+      <c r="C189" s="4">
+        <v>1</v>
+      </c>
       <c r="D189" s="4"/>
       <c r="E189" s="4" t="s">
         <v>526</v>
@@ -5289,7 +5406,9 @@
       <c r="B190" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C190" s="4"/>
+      <c r="C190" s="4">
+        <v>1</v>
+      </c>
       <c r="D190" s="4"/>
       <c r="E190" s="4" t="s">
         <v>527</v>
@@ -5302,7 +5421,9 @@
       <c r="B191" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C191" s="4"/>
+      <c r="C191" s="4">
+        <v>1</v>
+      </c>
       <c r="D191" s="4"/>
       <c r="E191" s="4" t="s">
         <v>528</v>
@@ -5315,7 +5436,9 @@
       <c r="B192" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C192" s="4"/>
+      <c r="C192" s="4">
+        <v>1</v>
+      </c>
       <c r="D192" s="4"/>
       <c r="E192" s="4" t="s">
         <v>529</v>
@@ -5328,7 +5451,9 @@
       <c r="B193" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C193" s="4"/>
+      <c r="C193" s="4">
+        <v>1</v>
+      </c>
       <c r="D193" s="4"/>
       <c r="E193" s="4" t="s">
         <v>530</v>
@@ -5341,7 +5466,9 @@
       <c r="B194" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C194" s="4"/>
+      <c r="C194" s="4">
+        <v>1</v>
+      </c>
       <c r="D194" s="4"/>
       <c r="E194" s="4" t="s">
         <v>531</v>
@@ -5354,7 +5481,9 @@
       <c r="B195" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C195" s="4"/>
+      <c r="C195" s="4">
+        <v>1</v>
+      </c>
       <c r="D195" s="4"/>
       <c r="E195" s="4" t="s">
         <v>581</v>
@@ -5367,7 +5496,9 @@
       <c r="B196" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C196" s="4"/>
+      <c r="C196" s="4">
+        <v>1</v>
+      </c>
       <c r="D196" s="4"/>
       <c r="E196" s="4" t="s">
         <v>532</v>
@@ -5380,7 +5511,9 @@
       <c r="B197" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C197" s="4"/>
+      <c r="C197" s="4">
+        <v>1</v>
+      </c>
       <c r="D197" s="4"/>
       <c r="E197" s="4" t="s">
         <v>533</v>
@@ -5393,7 +5526,9 @@
       <c r="B198" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C198" s="4"/>
+      <c r="C198" s="4">
+        <v>1</v>
+      </c>
       <c r="D198" s="4"/>
       <c r="E198" s="4" t="s">
         <v>534</v>
@@ -5406,7 +5541,9 @@
       <c r="B199" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C199" s="4"/>
+      <c r="C199" s="4">
+        <v>1</v>
+      </c>
       <c r="D199" s="4"/>
       <c r="E199" s="4" t="s">
         <v>535</v>
@@ -5419,7 +5556,9 @@
       <c r="B200" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C200" s="4"/>
+      <c r="C200" s="4">
+        <v>1</v>
+      </c>
       <c r="D200" s="4"/>
       <c r="E200" s="4" t="s">
         <v>536</v>
@@ -5432,7 +5571,9 @@
       <c r="B201" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C201" s="4"/>
+      <c r="C201" s="4">
+        <v>1</v>
+      </c>
       <c r="D201" s="4"/>
       <c r="E201" s="4" t="s">
         <v>537</v>
@@ -5445,7 +5586,9 @@
       <c r="B202" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C202" s="4"/>
+      <c r="C202" s="4">
+        <v>1</v>
+      </c>
       <c r="D202" s="4"/>
       <c r="E202" s="4" t="s">
         <v>538</v>
@@ -5458,7 +5601,9 @@
       <c r="B203" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C203" s="4"/>
+      <c r="C203" s="4">
+        <v>1</v>
+      </c>
       <c r="D203" s="4"/>
       <c r="E203" s="4" t="s">
         <v>539</v>
@@ -5471,7 +5616,9 @@
       <c r="B204" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C204" s="4"/>
+      <c r="C204" s="4">
+        <v>1</v>
+      </c>
       <c r="D204" s="4"/>
       <c r="E204" s="4" t="s">
         <v>540</v>
@@ -5484,7 +5631,9 @@
       <c r="B205" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C205" s="4"/>
+      <c r="C205" s="4">
+        <v>1</v>
+      </c>
       <c r="D205" s="4"/>
       <c r="E205" s="4" t="s">
         <v>541</v>
@@ -5497,7 +5646,9 @@
       <c r="B206" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C206" s="4"/>
+      <c r="C206" s="4">
+        <v>1</v>
+      </c>
       <c r="D206" s="4"/>
       <c r="E206" s="4" t="s">
         <v>542</v>
@@ -5510,7 +5661,9 @@
       <c r="B207" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C207" s="4"/>
+      <c r="C207" s="4">
+        <v>1</v>
+      </c>
       <c r="D207" s="4"/>
       <c r="E207" s="4" t="s">
         <v>543</v>
@@ -5523,7 +5676,9 @@
       <c r="B208" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C208" s="4"/>
+      <c r="C208" s="4">
+        <v>1</v>
+      </c>
       <c r="D208" s="4"/>
       <c r="E208" s="4" t="s">
         <v>544</v>
@@ -5572,7 +5727,9 @@
       <c r="B216" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C216" s="4"/>
+      <c r="C216" s="4">
+        <v>1</v>
+      </c>
       <c r="D216" s="4"/>
       <c r="E216" s="4" t="s">
         <v>181</v>
@@ -5585,7 +5742,9 @@
       <c r="B217" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C217" s="4"/>
+      <c r="C217" s="4">
+        <v>1</v>
+      </c>
       <c r="D217" s="4"/>
       <c r="E217" s="4" t="s">
         <v>183</v>
@@ -5598,7 +5757,9 @@
       <c r="B218" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C218" s="4"/>
+      <c r="C218" s="4">
+        <v>1</v>
+      </c>
       <c r="D218" s="4"/>
       <c r="E218" s="4" t="s">
         <v>185</v>
@@ -5611,7 +5772,9 @@
       <c r="B219" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C219" s="4"/>
+      <c r="C219" s="4">
+        <v>1</v>
+      </c>
       <c r="D219" s="4"/>
       <c r="E219" s="4" t="s">
         <v>187</v>
@@ -5624,7 +5787,9 @@
       <c r="B220" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C220" s="4"/>
+      <c r="C220" s="4">
+        <v>1</v>
+      </c>
       <c r="D220" s="4"/>
       <c r="E220" s="4" t="s">
         <v>189</v>
@@ -5637,7 +5802,9 @@
       <c r="B221" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C221" s="4"/>
+      <c r="C221" s="4">
+        <v>1</v>
+      </c>
       <c r="D221" s="4"/>
       <c r="E221" s="4" t="s">
         <v>191</v>
@@ -5650,7 +5817,9 @@
       <c r="B222" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C222" s="4"/>
+      <c r="C222" s="4">
+        <v>1</v>
+      </c>
       <c r="D222" s="4"/>
       <c r="E222" s="4" t="s">
         <v>545</v>
@@ -5663,7 +5832,9 @@
       <c r="B223" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C223" s="4"/>
+      <c r="C223" s="4">
+        <v>1</v>
+      </c>
       <c r="D223" s="4"/>
       <c r="E223" s="4" t="s">
         <v>194</v>
@@ -5676,7 +5847,9 @@
       <c r="B224" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C224" s="4"/>
+      <c r="C224" s="4">
+        <v>1</v>
+      </c>
       <c r="D224" s="4"/>
       <c r="E224" s="4" t="s">
         <v>196</v>
@@ -5689,7 +5862,9 @@
       <c r="B225" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C225" s="4"/>
+      <c r="C225" s="4">
+        <v>1</v>
+      </c>
       <c r="D225" s="4"/>
       <c r="E225" s="4" t="s">
         <v>198</v>
@@ -5702,7 +5877,9 @@
       <c r="B226" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C226" s="4"/>
+      <c r="C226" s="4">
+        <v>1</v>
+      </c>
       <c r="D226" s="4"/>
       <c r="E226" s="4" t="s">
         <v>200</v>
@@ -5715,7 +5892,9 @@
       <c r="B227" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C227" s="4"/>
+      <c r="C227" s="4">
+        <v>1</v>
+      </c>
       <c r="D227" s="4"/>
       <c r="E227" s="4" t="s">
         <v>202</v>
@@ -5728,7 +5907,9 @@
       <c r="B228" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C228" s="4"/>
+      <c r="C228" s="4">
+        <v>1</v>
+      </c>
       <c r="D228" s="4"/>
       <c r="E228" s="4" t="s">
         <v>204</v>
@@ -5783,7 +5964,9 @@
       <c r="B235" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C235" s="37"/>
+      <c r="C235" s="37">
+        <v>1</v>
+      </c>
       <c r="D235" s="37"/>
       <c r="E235" s="37" t="s">
         <v>692</v>
@@ -5838,7 +6021,9 @@
       <c r="B242" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C242" s="37"/>
+      <c r="C242" s="37">
+        <v>1</v>
+      </c>
       <c r="D242" s="37"/>
       <c r="E242" s="37" t="s">
         <v>699</v>
@@ -5886,7 +6071,9 @@
       <c r="B249" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C249" s="37"/>
+      <c r="C249" s="37">
+        <v>1</v>
+      </c>
       <c r="D249" s="37"/>
       <c r="E249" s="37" t="s">
         <v>701</v>
@@ -5929,7 +6116,9 @@
       <c r="B256" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C256" s="4"/>
+      <c r="C256" s="4">
+        <v>1</v>
+      </c>
       <c r="D256" s="4"/>
       <c r="E256" s="4" t="s">
         <v>208</v>
@@ -5942,7 +6131,9 @@
       <c r="B257" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C257" s="4"/>
+      <c r="C257" s="4">
+        <v>1</v>
+      </c>
       <c r="D257" s="4"/>
       <c r="E257" s="4" t="s">
         <v>210</v>
@@ -5955,7 +6146,9 @@
       <c r="B258" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C258" s="4"/>
+      <c r="C258" s="4">
+        <v>1</v>
+      </c>
       <c r="D258" s="4"/>
       <c r="E258" s="4" t="s">
         <v>212</v>
@@ -5968,7 +6161,9 @@
       <c r="B259" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C259" s="4"/>
+      <c r="C259" s="4">
+        <v>1</v>
+      </c>
       <c r="D259" s="4"/>
       <c r="E259" s="4" t="s">
         <v>214</v>
@@ -5981,7 +6176,9 @@
       <c r="B260" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C260" s="4"/>
+      <c r="C260" s="4">
+        <v>1</v>
+      </c>
       <c r="D260" s="4"/>
       <c r="E260" s="4" t="s">
         <v>216</v>
@@ -5994,7 +6191,9 @@
       <c r="B261" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C261" s="4"/>
+      <c r="C261" s="4">
+        <v>1</v>
+      </c>
       <c r="D261" s="4"/>
       <c r="E261" s="4" t="s">
         <v>218</v>
@@ -6007,7 +6206,9 @@
       <c r="B262" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C262" s="4"/>
+      <c r="C262" s="4">
+        <v>1</v>
+      </c>
       <c r="D262" s="4"/>
       <c r="E262" s="4" t="s">
         <v>220</v>
@@ -6020,7 +6221,9 @@
       <c r="B263" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C263" s="4"/>
+      <c r="C263" s="4">
+        <v>1</v>
+      </c>
       <c r="D263" s="4"/>
       <c r="E263" s="4" t="s">
         <v>222</v>
@@ -6033,7 +6236,9 @@
       <c r="B264" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C264" s="4"/>
+      <c r="C264" s="4">
+        <v>1</v>
+      </c>
       <c r="D264" s="4"/>
       <c r="E264" s="4" t="s">
         <v>224</v>
@@ -6046,7 +6251,9 @@
       <c r="B265" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C265" s="4"/>
+      <c r="C265" s="4">
+        <v>1</v>
+      </c>
       <c r="D265" s="4"/>
       <c r="E265" s="4" t="s">
         <v>226</v>
@@ -6059,7 +6266,9 @@
       <c r="B266" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C266" s="4"/>
+      <c r="C266" s="4">
+        <v>1</v>
+      </c>
       <c r="D266" s="4"/>
       <c r="E266" s="4" t="s">
         <v>228</v>
@@ -6072,7 +6281,9 @@
       <c r="B267" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C267" s="4"/>
+      <c r="C267" s="4">
+        <v>1</v>
+      </c>
       <c r="D267" s="4"/>
       <c r="E267" s="4" t="s">
         <v>230</v>
@@ -6085,8 +6296,12 @@
       <c r="B268" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C268" s="4"/>
-      <c r="D268" s="4"/>
+      <c r="C268" s="4">
+        <v>0</v>
+      </c>
+      <c r="D268" s="4" t="s">
+        <v>733</v>
+      </c>
       <c r="E268" s="4" t="s">
         <v>232</v>
       </c>
@@ -6098,8 +6313,12 @@
       <c r="B269" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C269" s="4"/>
-      <c r="D269" s="4"/>
+      <c r="C269" s="4">
+        <v>0</v>
+      </c>
+      <c r="D269" s="4" t="s">
+        <v>733</v>
+      </c>
       <c r="E269" s="4" t="s">
         <v>234</v>
       </c>
@@ -6111,7 +6330,9 @@
       <c r="B270" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C270" s="4"/>
+      <c r="C270" s="4">
+        <v>1</v>
+      </c>
       <c r="D270" s="4"/>
       <c r="E270" s="4" t="s">
         <v>546</v>
@@ -6124,7 +6345,9 @@
       <c r="B271" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C271" s="4"/>
+      <c r="C271" s="4">
+        <v>1</v>
+      </c>
       <c r="D271" s="4"/>
       <c r="E271" s="4" t="s">
         <v>547</v>
@@ -6137,7 +6360,9 @@
       <c r="B272" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C272" s="4"/>
+      <c r="C272" s="4">
+        <v>1</v>
+      </c>
       <c r="D272" s="4"/>
       <c r="E272" s="4" t="s">
         <v>548</v>
@@ -6150,8 +6375,12 @@
       <c r="B273" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C273" s="4"/>
-      <c r="D273" s="4"/>
+      <c r="C273" s="4">
+        <v>0</v>
+      </c>
+      <c r="D273" s="4" t="s">
+        <v>733</v>
+      </c>
       <c r="E273" s="4" t="s">
         <v>239</v>
       </c>
@@ -6163,7 +6392,9 @@
       <c r="B274" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C274" s="4"/>
+      <c r="C274" s="4">
+        <v>1</v>
+      </c>
       <c r="D274" s="4"/>
       <c r="E274" s="4" t="s">
         <v>241</v>
@@ -6176,7 +6407,9 @@
       <c r="B275" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C275" s="4"/>
+      <c r="C275" s="4">
+        <v>0</v>
+      </c>
       <c r="D275" s="4"/>
       <c r="E275" s="4" t="s">
         <v>243</v>
@@ -6189,7 +6422,9 @@
       <c r="B276" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C276" s="4"/>
+      <c r="C276" s="4">
+        <v>0</v>
+      </c>
       <c r="D276" s="4"/>
       <c r="E276" s="4" t="s">
         <v>245</v>
@@ -6202,7 +6437,9 @@
       <c r="B277" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C277" s="4"/>
+      <c r="C277" s="4">
+        <v>1</v>
+      </c>
       <c r="D277" s="4"/>
       <c r="E277" s="4" t="s">
         <v>247</v>
@@ -6215,7 +6452,9 @@
       <c r="B278" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C278" s="4"/>
+      <c r="C278" s="4">
+        <v>1</v>
+      </c>
       <c r="D278" s="4"/>
       <c r="E278" s="4" t="s">
         <v>249</v>
@@ -6228,7 +6467,9 @@
       <c r="B279" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C279" s="4"/>
+      <c r="C279" s="4">
+        <v>1</v>
+      </c>
       <c r="D279" s="4"/>
       <c r="E279" s="4" t="s">
         <v>251</v>
@@ -6241,7 +6482,9 @@
       <c r="B280" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C280" s="4"/>
+      <c r="C280" s="4">
+        <v>1</v>
+      </c>
       <c r="D280" s="4"/>
       <c r="E280" s="4" t="s">
         <v>253</v>
@@ -6254,7 +6497,9 @@
       <c r="B281" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C281" s="4"/>
+      <c r="C281" s="4">
+        <v>0</v>
+      </c>
       <c r="D281" s="4"/>
       <c r="E281" s="4" t="s">
         <v>255</v>
@@ -6267,7 +6512,9 @@
       <c r="B282" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C282" s="4"/>
+      <c r="C282" s="4">
+        <v>0</v>
+      </c>
       <c r="D282" s="4"/>
       <c r="E282" s="4" t="s">
         <v>257</v>
@@ -6280,7 +6527,9 @@
       <c r="B283" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C283" s="4"/>
+      <c r="C283" s="4">
+        <v>0</v>
+      </c>
       <c r="D283" s="4"/>
       <c r="E283" s="4" t="s">
         <v>259</v>
@@ -6324,7 +6573,9 @@
       <c r="B290" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C290" s="21"/>
+      <c r="C290" s="21">
+        <v>1</v>
+      </c>
       <c r="D290" s="4"/>
       <c r="E290" s="4" t="s">
         <v>614</v>
@@ -6337,7 +6588,9 @@
       <c r="B291" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C291" s="21"/>
+      <c r="C291" s="21">
+        <v>1</v>
+      </c>
       <c r="D291" s="4"/>
       <c r="E291" s="4" t="s">
         <v>264</v>
@@ -6350,7 +6603,9 @@
       <c r="B292" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C292" s="21"/>
+      <c r="C292" s="21">
+        <v>1</v>
+      </c>
       <c r="D292" s="4"/>
       <c r="E292" s="4" t="s">
         <v>266</v>
@@ -6363,7 +6618,9 @@
       <c r="B293" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C293" s="21"/>
+      <c r="C293" s="21">
+        <v>1</v>
+      </c>
       <c r="D293" s="4"/>
       <c r="E293" s="4" t="s">
         <v>268</v>
@@ -6376,7 +6633,9 @@
       <c r="B294" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C294" s="21"/>
+      <c r="C294" s="21">
+        <v>1</v>
+      </c>
       <c r="D294" s="4"/>
       <c r="E294" s="4" t="s">
         <v>270</v>
@@ -6389,7 +6648,9 @@
       <c r="B295" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C295" s="21"/>
+      <c r="C295" s="21">
+        <v>1</v>
+      </c>
       <c r="D295" s="4"/>
       <c r="E295" s="4" t="s">
         <v>272</v>
@@ -6402,7 +6663,9 @@
       <c r="B296" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C296" s="21"/>
+      <c r="C296" s="21">
+        <v>1</v>
+      </c>
       <c r="D296" s="4"/>
       <c r="E296" s="4" t="s">
         <v>274</v>
@@ -6415,7 +6678,9 @@
       <c r="B297" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C297" s="21"/>
+      <c r="C297" s="21">
+        <v>1</v>
+      </c>
       <c r="D297" s="4"/>
       <c r="E297" s="4" t="s">
         <v>276</v>
@@ -6428,7 +6693,9 @@
       <c r="B298" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C298" s="21"/>
+      <c r="C298" s="21">
+        <v>1</v>
+      </c>
       <c r="D298" s="4"/>
       <c r="E298" s="4" t="s">
         <v>278</v>
@@ -6441,7 +6708,9 @@
       <c r="B299" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C299" s="21"/>
+      <c r="C299" s="21">
+        <v>1</v>
+      </c>
       <c r="D299" s="4"/>
       <c r="E299" s="4" t="s">
         <v>280</v>
@@ -6454,7 +6723,9 @@
       <c r="B300" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C300" s="21"/>
+      <c r="C300" s="21">
+        <v>1</v>
+      </c>
       <c r="D300" s="4"/>
       <c r="E300" s="4" t="s">
         <v>282</v>
@@ -6467,7 +6738,9 @@
       <c r="B301" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C301" s="21"/>
+      <c r="C301" s="21">
+        <v>1</v>
+      </c>
       <c r="D301" s="4"/>
       <c r="E301" s="4" t="s">
         <v>284</v>
@@ -6480,7 +6753,9 @@
       <c r="B302" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C302" s="21"/>
+      <c r="C302" s="21">
+        <v>1</v>
+      </c>
       <c r="D302" s="4"/>
       <c r="E302" s="4" t="s">
         <v>286</v>
@@ -6493,7 +6768,9 @@
       <c r="B303" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C303" s="21"/>
+      <c r="C303" s="21">
+        <v>1</v>
+      </c>
       <c r="D303" s="4"/>
       <c r="E303" s="4" t="s">
         <v>288</v>
@@ -6506,7 +6783,9 @@
       <c r="B304" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C304" s="21"/>
+      <c r="C304" s="21">
+        <v>1</v>
+      </c>
       <c r="D304" s="4"/>
       <c r="E304" s="4" t="s">
         <v>615</v>
@@ -6519,7 +6798,9 @@
       <c r="B305" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C305" s="21"/>
+      <c r="C305" s="21">
+        <v>1</v>
+      </c>
       <c r="D305" s="4"/>
       <c r="E305" s="4" t="s">
         <v>291</v>
@@ -6532,7 +6813,9 @@
       <c r="B306" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C306" s="21"/>
+      <c r="C306" s="21">
+        <v>1</v>
+      </c>
       <c r="D306" s="4"/>
       <c r="E306" s="4" t="s">
         <v>293</v>
@@ -6545,7 +6828,9 @@
       <c r="B307" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C307" s="21"/>
+      <c r="C307" s="21">
+        <v>1</v>
+      </c>
       <c r="D307" s="4"/>
       <c r="E307" s="4" t="s">
         <v>295</v>
@@ -6558,7 +6843,9 @@
       <c r="B308" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C308" s="21"/>
+      <c r="C308" s="21">
+        <v>1</v>
+      </c>
       <c r="D308" s="4"/>
       <c r="E308" s="4" t="s">
         <v>549</v>
@@ -6571,7 +6858,9 @@
       <c r="B309" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C309" s="21"/>
+      <c r="C309" s="21">
+        <v>1</v>
+      </c>
       <c r="D309" s="4"/>
       <c r="E309" s="4" t="s">
         <v>298</v>
@@ -6584,7 +6873,9 @@
       <c r="B310" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C310" s="21"/>
+      <c r="C310" s="21">
+        <v>1</v>
+      </c>
       <c r="D310" s="4"/>
       <c r="E310" s="4" t="s">
         <v>300</v>
@@ -6597,7 +6888,9 @@
       <c r="B311" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C311" s="21"/>
+      <c r="C311" s="21">
+        <v>1</v>
+      </c>
       <c r="D311" s="4"/>
       <c r="E311" s="4" t="s">
         <v>550</v>
@@ -6610,7 +6903,9 @@
       <c r="B312" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C312" s="21"/>
+      <c r="C312" s="21">
+        <v>1</v>
+      </c>
       <c r="D312" s="4"/>
       <c r="E312" s="4" t="s">
         <v>303</v>
@@ -6623,7 +6918,9 @@
       <c r="B313" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C313" s="21"/>
+      <c r="C313" s="21">
+        <v>1</v>
+      </c>
       <c r="D313" s="4"/>
       <c r="E313" s="4" t="s">
         <v>305</v>
@@ -6636,7 +6933,9 @@
       <c r="B314" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C314" s="21"/>
+      <c r="C314" s="21">
+        <v>1</v>
+      </c>
       <c r="D314" s="4"/>
       <c r="E314" s="4" t="s">
         <v>307</v>
@@ -6649,7 +6948,9 @@
       <c r="B315" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C315" s="21"/>
+      <c r="C315" s="21">
+        <v>1</v>
+      </c>
       <c r="D315" s="4"/>
       <c r="E315" s="4" t="s">
         <v>309</v>
@@ -6662,7 +6963,9 @@
       <c r="B316" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C316" s="21"/>
+      <c r="C316" s="21">
+        <v>1</v>
+      </c>
       <c r="D316" s="4"/>
       <c r="E316" s="4" t="s">
         <v>311</v>
@@ -6675,7 +6978,9 @@
       <c r="B317" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C317" s="21"/>
+      <c r="C317" s="21">
+        <v>1</v>
+      </c>
       <c r="D317" s="4"/>
       <c r="E317" s="4" t="s">
         <v>313</v>
@@ -6688,7 +6993,9 @@
       <c r="B318" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C318" s="21"/>
+      <c r="C318" s="21">
+        <v>1</v>
+      </c>
       <c r="D318" s="4"/>
       <c r="E318" s="4" t="s">
         <v>315</v>
@@ -6701,7 +7008,9 @@
       <c r="B319" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C319" s="21"/>
+      <c r="C319" s="21">
+        <v>1</v>
+      </c>
       <c r="D319" s="4"/>
       <c r="E319" s="4" t="s">
         <v>317</v>
@@ -6714,7 +7023,9 @@
       <c r="B320" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C320" s="21"/>
+      <c r="C320" s="21">
+        <v>1</v>
+      </c>
       <c r="D320" s="4"/>
       <c r="E320" s="4" t="s">
         <v>319</v>
@@ -6727,7 +7038,9 @@
       <c r="B321" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C321" s="21"/>
+      <c r="C321" s="21">
+        <v>1</v>
+      </c>
       <c r="D321" s="4"/>
       <c r="E321" s="4" t="s">
         <v>321</v>
@@ -6740,7 +7053,9 @@
       <c r="B322" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C322" s="21"/>
+      <c r="C322" s="21">
+        <v>1</v>
+      </c>
       <c r="D322" s="4"/>
       <c r="E322" s="4" t="s">
         <v>323</v>
@@ -6753,7 +7068,9 @@
       <c r="B323" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C323" s="21"/>
+      <c r="C323" s="21">
+        <v>1</v>
+      </c>
       <c r="D323" s="4"/>
       <c r="E323" s="4" t="s">
         <v>325</v>
@@ -6766,7 +7083,9 @@
       <c r="B324" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C324" s="21"/>
+      <c r="C324" s="21">
+        <v>1</v>
+      </c>
       <c r="D324" s="4"/>
       <c r="E324" s="4" t="s">
         <v>327</v>
@@ -6779,7 +7098,9 @@
       <c r="B325" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C325" s="21"/>
+      <c r="C325" s="21">
+        <v>1</v>
+      </c>
       <c r="D325" s="4"/>
       <c r="E325" s="4" t="s">
         <v>329</v>
@@ -6792,7 +7113,9 @@
       <c r="B326" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C326" s="21"/>
+      <c r="C326" s="21">
+        <v>1</v>
+      </c>
       <c r="D326" s="4"/>
       <c r="E326" s="4" t="s">
         <v>331</v>
@@ -6805,7 +7128,9 @@
       <c r="B327" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C327" s="21"/>
+      <c r="C327" s="21">
+        <v>1</v>
+      </c>
       <c r="D327" s="4"/>
       <c r="E327" s="4" t="s">
         <v>333</v>
@@ -6818,7 +7143,9 @@
       <c r="B328" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C328" s="21"/>
+      <c r="C328" s="21">
+        <v>1</v>
+      </c>
       <c r="D328" s="4"/>
       <c r="E328" s="4" t="s">
         <v>335</v>
@@ -6831,7 +7158,9 @@
       <c r="B329" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C329" s="21"/>
+      <c r="C329" s="21">
+        <v>1</v>
+      </c>
       <c r="D329" s="4"/>
       <c r="E329" s="4" t="s">
         <v>337</v>
@@ -6844,7 +7173,9 @@
       <c r="B330" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C330" s="21"/>
+      <c r="C330" s="21">
+        <v>1</v>
+      </c>
       <c r="D330" s="4"/>
       <c r="E330" s="4" t="s">
         <v>339</v>
@@ -6857,7 +7188,9 @@
       <c r="B331" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C331" s="21"/>
+      <c r="C331" s="21">
+        <v>1</v>
+      </c>
       <c r="D331" s="4"/>
       <c r="E331" s="4" t="s">
         <v>341</v>
@@ -6906,7 +7239,9 @@
       <c r="B339" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C339" s="4"/>
+      <c r="C339" s="4">
+        <v>1</v>
+      </c>
       <c r="D339" s="4"/>
       <c r="E339" s="4" t="s">
         <v>346</v>
@@ -6919,7 +7254,9 @@
       <c r="B340" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C340" s="4"/>
+      <c r="C340" s="4">
+        <v>1</v>
+      </c>
       <c r="D340" s="4"/>
       <c r="E340" s="4" t="s">
         <v>348</v>
@@ -6932,8 +7269,12 @@
       <c r="B341" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C341" s="4"/>
-      <c r="D341" s="4"/>
+      <c r="C341" s="4">
+        <v>0</v>
+      </c>
+      <c r="D341" s="4" t="s">
+        <v>733</v>
+      </c>
       <c r="E341" s="4" t="s">
         <v>350</v>
       </c>
@@ -6945,8 +7286,12 @@
       <c r="B342" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C342" s="4"/>
-      <c r="D342" s="4"/>
+      <c r="C342" s="4">
+        <v>0</v>
+      </c>
+      <c r="D342" s="4" t="s">
+        <v>733</v>
+      </c>
       <c r="E342" s="4" t="s">
         <v>352</v>
       </c>
@@ -6958,8 +7303,12 @@
       <c r="B343" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C343" s="4"/>
-      <c r="D343" s="4"/>
+      <c r="C343" s="4">
+        <v>0</v>
+      </c>
+      <c r="D343" s="4" t="s">
+        <v>733</v>
+      </c>
       <c r="E343" s="4" t="s">
         <v>354</v>
       </c>
@@ -6971,8 +7320,12 @@
       <c r="B344" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C344" s="4"/>
-      <c r="D344" s="4"/>
+      <c r="C344" s="4">
+        <v>0</v>
+      </c>
+      <c r="D344" s="4" t="s">
+        <v>733</v>
+      </c>
       <c r="E344" s="4" t="s">
         <v>356</v>
       </c>
@@ -6993,7 +7346,9 @@
       <c r="B346" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C346" s="4"/>
+      <c r="C346" s="4">
+        <v>1</v>
+      </c>
       <c r="D346" s="4"/>
       <c r="E346" s="4" t="s">
         <v>359</v>
@@ -7033,7 +7388,9 @@
       <c r="B353" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C353" s="4"/>
+      <c r="C353" s="4">
+        <v>1</v>
+      </c>
       <c r="D353" s="4"/>
       <c r="E353" s="4" t="s">
         <v>551</v>
@@ -7046,7 +7403,9 @@
       <c r="B354" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C354" s="4"/>
+      <c r="C354" s="4">
+        <v>1</v>
+      </c>
       <c r="D354" s="4"/>
       <c r="E354" s="4" t="s">
         <v>552</v>
@@ -7059,7 +7418,9 @@
       <c r="B355" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C355" s="4"/>
+      <c r="C355" s="4">
+        <v>1</v>
+      </c>
       <c r="D355" s="4"/>
       <c r="E355" s="4" t="s">
         <v>553</v>
@@ -7072,7 +7433,9 @@
       <c r="B356" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C356" s="4"/>
+      <c r="C356" s="4">
+        <v>0</v>
+      </c>
       <c r="D356" s="4"/>
       <c r="E356" s="4" t="s">
         <v>554</v>
@@ -7085,7 +7448,9 @@
       <c r="B357" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C357" s="4"/>
+      <c r="C357" s="4">
+        <v>0</v>
+      </c>
       <c r="D357" s="4"/>
       <c r="E357" s="4" t="s">
         <v>555</v>
@@ -7098,7 +7463,9 @@
       <c r="B358" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C358" s="4"/>
+      <c r="C358" s="4">
+        <v>0</v>
+      </c>
       <c r="D358" s="4"/>
       <c r="E358" s="4" t="s">
         <v>556</v>
@@ -7111,7 +7478,9 @@
       <c r="B359" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C359" s="4"/>
+      <c r="C359" s="4">
+        <v>1</v>
+      </c>
       <c r="D359" s="4"/>
       <c r="E359" s="4" t="s">
         <v>557</v>
@@ -7124,7 +7493,9 @@
       <c r="B360" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C360" s="4"/>
+      <c r="C360" s="4">
+        <v>1</v>
+      </c>
       <c r="D360" s="4"/>
       <c r="E360" s="4" t="s">
         <v>558</v>
@@ -7137,7 +7508,9 @@
       <c r="B361" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C361" s="4"/>
+      <c r="C361" s="4">
+        <v>1</v>
+      </c>
       <c r="D361" s="4"/>
       <c r="E361" s="4" t="s">
         <v>559</v>
@@ -7150,7 +7523,9 @@
       <c r="B362" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C362" s="4"/>
+      <c r="C362" s="4">
+        <v>1</v>
+      </c>
       <c r="D362" s="4"/>
       <c r="E362" s="4" t="s">
         <v>560</v>
@@ -7163,7 +7538,9 @@
       <c r="B363" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C363" s="4"/>
+      <c r="C363" s="4">
+        <v>1</v>
+      </c>
       <c r="D363" s="4"/>
       <c r="E363" s="4" t="s">
         <v>561</v>
@@ -7176,7 +7553,9 @@
       <c r="B364" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C364" s="4"/>
+      <c r="C364" s="4">
+        <v>1</v>
+      </c>
       <c r="D364" s="4"/>
       <c r="E364" s="4" t="s">
         <v>562</v>
@@ -7216,7 +7595,9 @@
       <c r="B371" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C371" s="4"/>
+      <c r="C371" s="4">
+        <v>1</v>
+      </c>
       <c r="D371" s="4"/>
       <c r="E371" s="4" t="s">
         <v>563</v>
@@ -7256,7 +7637,9 @@
       <c r="B378" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C378" s="4"/>
+      <c r="C378" s="4">
+        <v>1</v>
+      </c>
       <c r="D378" s="4"/>
       <c r="E378" s="4" t="s">
         <v>564</v>
@@ -7296,7 +7679,9 @@
       <c r="B385" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C385" s="4"/>
+      <c r="C385" s="4">
+        <v>0</v>
+      </c>
       <c r="D385" s="4"/>
       <c r="E385" s="4" t="s">
         <v>565</v>
@@ -7336,7 +7721,9 @@
       <c r="B392" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C392" s="4"/>
+      <c r="C392" s="4">
+        <v>1</v>
+      </c>
       <c r="D392" s="4"/>
       <c r="E392" s="4" t="s">
         <v>566</v>
@@ -7383,7 +7770,9 @@
       <c r="B399" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C399" s="4"/>
+      <c r="C399" s="4">
+        <v>1</v>
+      </c>
       <c r="D399" s="4"/>
       <c r="E399" s="4" t="s">
         <v>567</v>
@@ -7423,7 +7812,9 @@
       <c r="B406" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C406" s="4"/>
+      <c r="C406" s="4">
+        <v>1</v>
+      </c>
       <c r="D406" s="4"/>
       <c r="E406" s="4" t="s">
         <v>568</v>
@@ -7463,7 +7854,9 @@
       <c r="B413" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C413" s="4"/>
+      <c r="C413" s="4">
+        <v>1</v>
+      </c>
       <c r="D413" s="4"/>
       <c r="E413" s="4" t="s">
         <v>569</v>
@@ -7503,7 +7896,9 @@
       <c r="B420" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C420" s="4"/>
+      <c r="C420" s="4">
+        <v>1</v>
+      </c>
       <c r="D420" s="4"/>
       <c r="E420" s="4" t="s">
         <v>570</v>
@@ -7543,7 +7938,9 @@
       <c r="B427" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C427" s="4"/>
+      <c r="C427" s="4">
+        <v>1</v>
+      </c>
       <c r="D427" s="4"/>
       <c r="E427" s="4" t="s">
         <v>571</v>
@@ -7590,7 +7987,9 @@
       <c r="B434" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C434" s="4"/>
+      <c r="C434" s="4">
+        <v>0</v>
+      </c>
       <c r="D434" s="4"/>
       <c r="E434" s="4" t="s">
         <v>572</v>
@@ -7603,7 +8002,9 @@
       <c r="B435" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C435" s="4"/>
+      <c r="C435" s="4">
+        <v>0</v>
+      </c>
       <c r="D435" s="4"/>
       <c r="E435" s="4" t="s">
         <v>573</v>
@@ -7643,7 +8044,9 @@
       <c r="B442" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C442" s="4"/>
+      <c r="C442" s="4">
+        <v>1</v>
+      </c>
       <c r="D442" s="4"/>
       <c r="E442" s="4" t="s">
         <v>407</v>
@@ -7656,7 +8059,9 @@
       <c r="B443" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C443" s="4"/>
+      <c r="C443" s="4">
+        <v>0</v>
+      </c>
       <c r="D443" s="4"/>
       <c r="E443" s="4" t="s">
         <v>409</v>
@@ -7669,7 +8074,9 @@
       <c r="B444" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C444" s="4"/>
+      <c r="C444" s="4">
+        <v>0</v>
+      </c>
       <c r="D444" s="4"/>
       <c r="E444" s="4" t="s">
         <v>411</v>
@@ -7682,7 +8089,9 @@
       <c r="B445" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C445" s="4"/>
+      <c r="C445" s="4">
+        <v>1</v>
+      </c>
       <c r="D445" s="4"/>
       <c r="E445" s="4" t="s">
         <v>413</v>
@@ -7722,7 +8131,9 @@
       <c r="B452" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C452" s="4"/>
+      <c r="C452" s="4">
+        <v>1</v>
+      </c>
       <c r="D452" s="4"/>
       <c r="E452" s="4" t="s">
         <v>208</v>
@@ -7735,7 +8146,9 @@
       <c r="B453" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C453" s="4"/>
+      <c r="C453" s="4">
+        <v>1</v>
+      </c>
       <c r="D453" s="4"/>
       <c r="E453" s="4" t="s">
         <v>210</v>
@@ -7748,7 +8161,9 @@
       <c r="B454" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C454" s="4"/>
+      <c r="C454" s="4">
+        <v>1</v>
+      </c>
       <c r="D454" s="4"/>
       <c r="E454" s="4" t="s">
         <v>212</v>
@@ -7761,7 +8176,9 @@
       <c r="B455" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C455" s="4"/>
+      <c r="C455" s="4">
+        <v>1</v>
+      </c>
       <c r="D455" s="4"/>
       <c r="E455" s="4" t="s">
         <v>214</v>
@@ -7774,7 +8191,9 @@
       <c r="B456" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C456" s="4"/>
+      <c r="C456" s="4">
+        <v>1</v>
+      </c>
       <c r="D456" s="4"/>
       <c r="E456" s="4" t="s">
         <v>216</v>
@@ -7787,7 +8206,9 @@
       <c r="B457" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C457" s="4"/>
+      <c r="C457" s="4">
+        <v>1</v>
+      </c>
       <c r="D457" s="4"/>
       <c r="E457" s="4" t="s">
         <v>218</v>
@@ -7800,7 +8221,9 @@
       <c r="B458" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C458" s="4"/>
+      <c r="C458" s="4">
+        <v>1</v>
+      </c>
       <c r="D458" s="4"/>
       <c r="E458" s="4" t="s">
         <v>232</v>
@@ -7813,7 +8236,9 @@
       <c r="B459" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C459" s="4"/>
+      <c r="C459" s="4">
+        <v>0</v>
+      </c>
       <c r="D459" s="4"/>
       <c r="E459" s="4" t="s">
         <v>234</v>
@@ -7826,7 +8251,9 @@
       <c r="B460" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C460" s="4"/>
+      <c r="C460" s="4">
+        <v>1</v>
+      </c>
       <c r="D460" s="4"/>
       <c r="E460" s="4" t="s">
         <v>425</v>
@@ -7839,7 +8266,9 @@
       <c r="B461" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C461" s="4"/>
+      <c r="C461" s="4">
+        <v>1</v>
+      </c>
       <c r="D461" s="4"/>
       <c r="E461" s="4" t="s">
         <v>259</v>

</xml_diff>